<commit_message>
Define KVS Table definition xlsx and xml for meta2xml.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoKeyGeneratorKtSample.xlsx
+++ b/meta/objects/BlancoKeyGeneratorKtSample.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoKeyGeneratorKt/meta/objects/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E328748-1F9A-7247-9D34-15588A68E203}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C21F0C-3A94-9B43-993C-87B0B6E15AB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6860" yWindow="1180" windowWidth="25440" windowHeight="18580" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3100" yWindow="1240" windowWidth="35380" windowHeight="18580" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tabale v.1" sheetId="1" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="109">
   <si>
     <t>クラス名</t>
   </si>
@@ -207,12 +207,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>@JsonAutoDetect(
-    "hoge: fuga")
-@NotNull</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>総称型</t>
     <rPh sb="0" eb="3">
       <t xml:space="preserve">ソウショウガタ </t>
@@ -220,10 +214,6 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>T</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>1.このキー定義書は、blancoKeyGeneratorが入力ファイルとして利用します。</t>
     <phoneticPr fontId="4"/>
   </si>
@@ -300,19 +290,6 @@
   </si>
   <si>
     <t>キー定義書のサンプル。このクラスは単にサンプルです。実際の動作には利用されません。</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
-    <t>アノテーション付きキー定義書のサンプル。アノテーションは2重のバックスラッシュ区切りで複数記述できます。このクラスは単にサンプルです。実際の動作には利用されません。</t>
-    <rPh sb="7" eb="8">
-      <t>ツキ</t>
-    </rPh>
-    <rPh sb="35" eb="37">
-      <t>フクスウ</t>
-    </rPh>
-    <rPh sb="37" eb="39">
-      <t>キジュツ</t>
-    </rPh>
     <phoneticPr fontId="4"/>
   </si>
   <si>
@@ -2181,8 +2158,8 @@
   </sheetPr>
   <dimension ref="A1:O60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39:F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -2199,14 +2176,14 @@
     <col min="10" max="10" width="16.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.1640625" style="1" customWidth="1"/>
     <col min="12" max="12" width="6.83203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="28" style="1" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" style="1" customWidth="1"/>
     <col min="14" max="14" width="33.33203125" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="19">
       <c r="A1" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>12</v>
@@ -2214,12 +2191,12 @@
     </row>
     <row r="2" spans="1:13">
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:13">
@@ -2227,7 +2204,7 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="77" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -2245,7 +2222,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="12"/>
@@ -2262,7 +2239,7 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D7" s="29"/>
       <c r="E7" s="29"/>
@@ -2279,7 +2256,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D8" s="29"/>
       <c r="E8" s="29"/>
@@ -2292,12 +2269,10 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="10" t="s">
-        <v>32</v>
-      </c>
+      <c r="C9" s="10"/>
       <c r="D9" s="29"/>
       <c r="E9" s="29"/>
       <c r="F9" s="11"/>
@@ -2306,14 +2281,12 @@
       <c r="I9" s="30"/>
       <c r="K9" s="31"/>
     </row>
-    <row r="10" spans="1:13" ht="45">
+    <row r="10" spans="1:13">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="6"/>
-      <c r="C10" s="63" t="s">
-        <v>30</v>
-      </c>
+      <c r="C10" s="63"/>
       <c r="D10" s="29"/>
       <c r="E10" s="29"/>
       <c r="F10" s="11"/>
@@ -2329,7 +2302,7 @@
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="79" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D11" s="80"/>
       <c r="E11" s="80"/>
@@ -2348,7 +2321,7 @@
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="12"/>
@@ -2363,11 +2336,11 @@
     </row>
     <row r="13" spans="1:13" s="28" customFormat="1">
       <c r="A13" s="53" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B13" s="54"/>
       <c r="C13" s="55" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13"/>
       <c r="E13"/>
@@ -2380,14 +2353,14 @@
     </row>
     <row r="14" spans="1:13" s="28" customFormat="1">
       <c r="A14" s="53" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14" s="54"/>
       <c r="C14" s="55">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
@@ -2399,7 +2372,7 @@
     </row>
     <row r="15" spans="1:13" s="28" customFormat="1">
       <c r="A15" s="53" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B15" s="54"/>
       <c r="C15" s="55">
@@ -2416,7 +2389,7 @@
     </row>
     <row r="16" spans="1:13" s="28" customFormat="1">
       <c r="A16" s="53" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B16" s="54"/>
       <c r="C16" s="55">
@@ -2433,14 +2406,14 @@
     </row>
     <row r="17" spans="1:15" s="28" customFormat="1">
       <c r="A17" s="53" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B17" s="54"/>
       <c r="C17" s="55">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E17"/>
       <c r="F17"/>
@@ -2452,14 +2425,14 @@
     </row>
     <row r="18" spans="1:15" s="28" customFormat="1">
       <c r="A18" s="53" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B18" s="54"/>
       <c r="C18" s="55">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E18"/>
       <c r="F18"/>
@@ -2486,7 +2459,7 @@
     </row>
     <row r="20" spans="1:15">
       <c r="A20" s="26" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B20" s="27"/>
       <c r="C20" s="27"/>
@@ -2595,7 +2568,7 @@
     </row>
     <row r="26" spans="1:15">
       <c r="A26" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B26" s="14"/>
       <c r="C26" s="14"/>
@@ -2632,16 +2605,16 @@
         <v>6</v>
       </c>
       <c r="G27" s="86" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="H27" s="83" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="I27" s="86" t="s">
         <v>26</v>
       </c>
       <c r="J27" s="83" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="K27" s="82" t="s">
         <v>2</v>
@@ -2673,7 +2646,7 @@
         <v>1</v>
       </c>
       <c r="B29" s="20" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C29" s="21" t="s">
         <v>7</v>
@@ -2681,10 +2654,10 @@
       <c r="D29" s="21"/>
       <c r="E29" s="21"/>
       <c r="F29" s="21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="G29" s="61" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H29" s="61"/>
       <c r="I29" s="61" t="s">
@@ -2694,7 +2667,7 @@
         <v>10</v>
       </c>
       <c r="K29" s="21" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="L29" s="22"/>
       <c r="M29" s="22"/>
@@ -2707,7 +2680,7 @@
         <v>2</v>
       </c>
       <c r="B30" s="20" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C30" s="21" t="s">
         <v>25</v>
@@ -2718,7 +2691,7 @@
         <v>0</v>
       </c>
       <c r="G30" s="61" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H30" s="61"/>
       <c r="I30" s="61" t="s">
@@ -2728,7 +2701,7 @@
         <v>64</v>
       </c>
       <c r="K30" s="21" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="L30" s="22"/>
       <c r="M30" s="22"/>
@@ -2741,7 +2714,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="20" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C31" s="21" t="s">
         <v>25</v>
@@ -2752,7 +2725,7 @@
         <v>0</v>
       </c>
       <c r="G31" s="61" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="H31" s="61"/>
       <c r="I31" s="61" t="s">
@@ -2762,7 +2735,7 @@
         <v>64</v>
       </c>
       <c r="K31" s="21" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L31" s="22"/>
       <c r="M31" s="22"/>
@@ -2775,7 +2748,7 @@
         <v>4</v>
       </c>
       <c r="B32" s="20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C32" s="21" t="s">
         <v>13</v>
@@ -2783,7 +2756,7 @@
       <c r="D32" s="21"/>
       <c r="E32" s="64"/>
       <c r="F32" s="21" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="G32" s="61"/>
       <c r="H32" s="61"/>
@@ -2794,7 +2767,7 @@
         <v>10</v>
       </c>
       <c r="K32" s="21" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="L32" s="22"/>
       <c r="M32" s="22"/>
@@ -2807,7 +2780,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C33" s="21" t="s">
         <v>9</v>
@@ -2815,14 +2788,14 @@
       <c r="D33" s="21"/>
       <c r="E33" s="62"/>
       <c r="F33" s="21" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G33" s="61"/>
       <c r="H33" s="61"/>
       <c r="I33" s="61"/>
       <c r="J33" s="21"/>
       <c r="K33" s="21" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="L33" s="22"/>
       <c r="M33" s="22"/>
@@ -2882,7 +2855,7 @@
     </row>
     <row r="38" spans="1:15">
       <c r="A38" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B38" s="14"/>
       <c r="C38" s="14"/>
@@ -2903,16 +2876,16 @@
         <v>14</v>
       </c>
       <c r="B39" s="78" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C39" s="97" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D39" s="99"/>
       <c r="E39" s="99"/>
       <c r="F39" s="100"/>
       <c r="G39" s="95" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H39" s="16"/>
       <c r="I39" s="16"/>
@@ -2945,22 +2918,22 @@
         <v>1</v>
       </c>
       <c r="B41" s="20" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C41" s="104" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D41" s="105"/>
       <c r="E41" s="105"/>
       <c r="F41" s="106"/>
       <c r="G41" s="92" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="H41" s="90"/>
       <c r="I41" s="90"/>
       <c r="J41" s="90"/>
       <c r="K41" s="21" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="L41" s="22"/>
       <c r="M41" s="90"/>
@@ -2972,22 +2945,22 @@
         <v>2</v>
       </c>
       <c r="B42" s="20" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C42" s="103" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D42" s="110"/>
       <c r="E42" s="110"/>
       <c r="F42" s="111"/>
       <c r="G42" s="93" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H42" s="90"/>
       <c r="I42" s="90"/>
       <c r="J42" s="90"/>
       <c r="K42" s="21" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L42" s="22"/>
       <c r="M42" s="90"/>
@@ -2999,22 +2972,22 @@
         <v>3</v>
       </c>
       <c r="B43" s="20" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C43" s="103" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D43" s="110"/>
       <c r="E43" s="110"/>
       <c r="F43" s="111"/>
       <c r="G43" s="93" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="H43" s="22"/>
       <c r="I43" s="22"/>
       <c r="J43" s="22"/>
       <c r="K43" s="21" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L43" s="22"/>
       <c r="M43" s="22"/>
@@ -3026,32 +2999,29 @@
         <v>4</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C44" s="103" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="D44" s="110"/>
       <c r="E44" s="110"/>
       <c r="F44" s="111"/>
       <c r="G44" s="93" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="H44" s="22"/>
       <c r="I44" s="22"/>
       <c r="J44" s="22"/>
       <c r="K44" s="21" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="L44" s="22"/>
       <c r="M44" s="22"/>
       <c r="N44" s="23"/>
     </row>
     <row r="45" spans="1:15">
-      <c r="A45" s="19">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
+      <c r="A45" s="19"/>
       <c r="B45" s="20"/>
       <c r="C45" s="103"/>
       <c r="D45" s="110"/>
@@ -3067,10 +3037,7 @@
       <c r="N45" s="23"/>
     </row>
     <row r="46" spans="1:15">
-      <c r="A46" s="19">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
+      <c r="A46" s="19"/>
       <c r="B46" s="76"/>
       <c r="C46" s="103"/>
       <c r="D46" s="110"/>
@@ -3086,10 +3053,7 @@
       <c r="N46" s="23"/>
     </row>
     <row r="47" spans="1:15">
-      <c r="A47" s="19">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
+      <c r="A47" s="19"/>
       <c r="B47" s="76"/>
       <c r="C47" s="103"/>
       <c r="D47" s="110"/>
@@ -3122,78 +3086,78 @@
     </row>
     <row r="50" spans="1:3">
       <c r="A50" s="1" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:3">
       <c r="A51" s="1" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="52" spans="1:3">
       <c r="B52" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:3">
       <c r="B53" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="B54" s="1" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="55" spans="1:3">
       <c r="B55" s="1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="56" spans="1:3">
       <c r="B56" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="58" spans="1:3">
       <c r="A58" s="1" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="59" spans="1:3">
       <c r="B59" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C59" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:3">
       <c r="B60" s="1" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -3309,10 +3273,10 @@
     </row>
     <row r="3" spans="1:17">
       <c r="B3" s="49" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F3" s="49" t="s">
         <v>28</v>
@@ -3335,10 +3299,10 @@
     </row>
     <row r="4" spans="1:17">
       <c r="B4" s="50" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D4" s="52" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F4" s="51" t="s">
         <v>29</v>
@@ -3351,10 +3315,10 @@
     </row>
     <row r="5" spans="1:17">
       <c r="B5" s="88" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D5" s="52" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F5" s="52"/>
       <c r="H5" s="52" t="s">
@@ -3375,7 +3339,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="B6" s="89" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>